<commit_message>
Stata code update + R Re-write
</commit_message>
<xml_diff>
--- a/results/Table2.xlsx
+++ b/results/Table2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1782CC5E-7A80-4F8B-9309-BD474229232B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2 combo AGI, panel A" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Table 2a (IRS) (Migr=AGI)" sheetId="5" r:id="rId8"/>
     <sheet name="Table 2b (ACS) (Migr = income)" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1712" uniqueCount="62">
   <si>
     <t>state_name</t>
   </si>
@@ -254,11 +254,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -330,34 +330,34 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,7 +530,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -554,9 +554,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -580,7 +580,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -615,7 +615,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -633,7 +633,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -658,7 +658,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -694,19 +694,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5E1998-FEE5-4295-B385-5E9C33FCE498}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5E1998-FEE5-4295-B385-5E9C33FCE498}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="12" t="s">
         <v>50</v>
@@ -758,7 +758,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -793,7 +793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -840,7 +840,7 @@
       </c>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
         <v>5.6045219302177429E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -947,7 +947,7 @@
         <v>5.4175112396478653E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -992,7 +992,7 @@
         <v>5.0596162676811218E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>4.6159025281667709E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="G14" s="6"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1149,7 +1149,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>4.99735027551651E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1239,10 +1239,10 @@
         <v>5.0142049789428711E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1252,7 +1252,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1262,10 +1262,10 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1273,10 +1273,10 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1284,7 +1284,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1292,7 +1292,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1300,7 +1300,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1308,7 +1308,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1316,13 +1316,13 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1330,7 +1330,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1338,13 +1338,13 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="34" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1352,7 +1352,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="35" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1388,17 +1388,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040F1D01-251C-4DA9-9CB9-0D8D107490A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040F1D01-251C-4DA9-9CB9-0D8D107490A2}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="12" t="s">
         <v>50</v>
@@ -1450,7 +1450,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>6.5405286848545074E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>5.9880614280700684E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>5.194174125790596E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>4.8938725143671036E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1833,7 +1833,7 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="G14" s="6"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1841,7 +1841,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>4.4156964868307114E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1931,10 +1931,10 @@
         <v>5.5787641555070877E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1944,7 +1944,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1954,10 +1954,10 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1965,10 +1965,10 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1976,7 +1976,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1984,7 +1984,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1992,7 +1992,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -2000,7 +2000,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -2008,13 +2008,13 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2022,7 +2022,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -2030,13 +2030,13 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="34" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2044,7 +2044,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="35" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2080,24 +2080,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEEC53B-99A0-4433-B7F2-5FB3FA503E7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEEC53B-99A0-4433-B7F2-5FB3FA503E7D}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
@@ -2117,7 +2117,7 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="C3" s="7" t="s">
         <v>55</v>
@@ -2143,12 +2143,12 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2178,13 +2178,13 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>-8.8994503021240234E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>-2.7064234018325806E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>-3.7825144827365875E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="E12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>9.4592086970806122E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2372,13 +2372,13 @@
       </c>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2454,16 +2454,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2503,25 +2503,25 @@
         <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>8.6629293859004974E-2</v>
+        <v>0.086629293859004974</v>
       </c>
       <c r="E2" s="1">
-        <v>8.8014185428619385E-2</v>
+        <v>0.088014185428619385</v>
       </c>
       <c r="F2" s="1">
-        <v>7.3985382914543152E-2</v>
+        <v>0.073985382914543152</v>
       </c>
       <c r="G2" s="1">
-        <v>7.5574591755867004E-2</v>
+        <v>0.075574591755867004</v>
       </c>
       <c r="H2" s="1">
-        <v>6.7215822637081146E-2</v>
+        <v>0.067215822637081146</v>
       </c>
       <c r="I2" s="1">
-        <v>8.1016130745410919E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.081016130745410919</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2532,25 +2532,25 @@
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>8.1532232463359833E-2</v>
+        <v>0.081532232463359833</v>
       </c>
       <c r="E3" s="1">
-        <v>8.7921030819416046E-2</v>
+        <v>0.087921030819416046</v>
       </c>
       <c r="F3" s="1">
-        <v>6.7221365869045258E-2</v>
+        <v>0.067221365869045258</v>
       </c>
       <c r="G3" s="1">
-        <v>7.4698098003864288E-2</v>
+        <v>0.074698098003864288</v>
       </c>
       <c r="H3" s="1">
-        <v>5.8235693722963333E-2</v>
+        <v>0.058235693722963333</v>
       </c>
       <c r="I3" s="1">
-        <v>6.4857304096221924E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.064857304096221924</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2561,25 +2561,25 @@
         <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>7.2237491607666016E-2</v>
+        <v>0.072237491607666016</v>
       </c>
       <c r="E4" s="1">
-        <v>8.0506063997745514E-2</v>
+        <v>0.080506063997745514</v>
       </c>
       <c r="F4" s="1">
-        <v>6.4522705972194672E-2</v>
+        <v>0.064522705972194672</v>
       </c>
       <c r="G4" s="1">
-        <v>7.3486529290676117E-2</v>
+        <v>0.073486529290676117</v>
       </c>
       <c r="H4" s="1">
-        <v>5.9354282915592194E-2</v>
+        <v>0.059354282915592194</v>
       </c>
       <c r="I4" s="1">
-        <v>6.6666498780250549E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.066666498780250549</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2590,25 +2590,25 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>6.5852485597133636E-2</v>
+        <v>0.065852485597133636</v>
       </c>
       <c r="E5" s="1">
-        <v>7.8191906213760376E-2</v>
+        <v>0.078191906213760376</v>
       </c>
       <c r="F5" s="1">
-        <v>5.9850100427865982E-2</v>
+        <v>0.059850100427865982</v>
       </c>
       <c r="G5" s="1">
-        <v>6.9575287401676178E-2</v>
+        <v>0.069575287401676178</v>
       </c>
       <c r="H5" s="1">
-        <v>5.2635479718446732E-2</v>
+        <v>0.052635479718446732</v>
       </c>
       <c r="I5" s="1">
-        <v>6.325937807559967E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.06325937807559967</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2619,25 +2619,25 @@
         <v>20</v>
       </c>
       <c r="D6" s="1">
-        <v>6.7704752087593079E-2</v>
+        <v>0.067704752087593079</v>
       </c>
       <c r="E6" s="1">
-        <v>6.8800784647464752E-2</v>
+        <v>0.068800784647464752</v>
       </c>
       <c r="F6" s="1">
-        <v>5.8075003325939178E-2</v>
+        <v>0.058075003325939178</v>
       </c>
       <c r="G6" s="1">
-        <v>5.6241076439619064E-2</v>
+        <v>0.056241076439619064</v>
       </c>
       <c r="H6" s="1">
-        <v>5.4442763328552246E-2</v>
+        <v>0.054442763328552246</v>
       </c>
       <c r="I6" s="1">
-        <v>5.3673293441534042E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.053673293441534042</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2648,25 +2648,25 @@
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>6.0768041759729385E-2</v>
+        <v>0.060768041759729385</v>
       </c>
       <c r="E7" s="1">
-        <v>6.7371338605880737E-2</v>
+        <v>0.067371338605880737</v>
       </c>
       <c r="F7" s="1">
-        <v>5.1399365067481995E-2</v>
+        <v>0.051399365067481995</v>
       </c>
       <c r="G7" s="1">
-        <v>5.6492134928703308E-2</v>
+        <v>0.056492134928703308</v>
       </c>
       <c r="H7" s="1">
-        <v>5.2986618131399155E-2</v>
+        <v>0.052986618131399155</v>
       </c>
       <c r="I7" s="1">
-        <v>5.1667891442775726E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.051667891442775726</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2677,25 +2677,25 @@
         <v>20</v>
       </c>
       <c r="D8" s="1">
-        <v>9.6729584038257599E-2</v>
+        <v>0.096729584038257599</v>
       </c>
       <c r="E8" s="1">
-        <v>8.497629314661026E-2</v>
+        <v>0.08497629314661026</v>
       </c>
       <c r="F8" s="1">
-        <v>8.6240604519844055E-2</v>
+        <v>0.086240604519844055</v>
       </c>
       <c r="G8" s="1">
-        <v>6.7156009376049042E-2</v>
+        <v>0.067156009376049042</v>
       </c>
       <c r="H8" s="1">
-        <v>9.6766941249370575E-2</v>
+        <v>0.096766941249370575</v>
       </c>
       <c r="I8" s="1">
-        <v>6.274983286857605E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.06274983286857605</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2706,25 +2706,25 @@
         <v>13</v>
       </c>
       <c r="D9" s="1">
-        <v>8.5019595921039581E-2</v>
+        <v>0.085019595921039581</v>
       </c>
       <c r="E9" s="1">
-        <v>8.763287216424942E-2</v>
+        <v>0.08763287216424942</v>
       </c>
       <c r="F9" s="1">
-        <v>7.3795154690742493E-2</v>
+        <v>0.073795154690742493</v>
       </c>
       <c r="G9" s="1">
-        <v>6.9099433720111847E-2</v>
+        <v>0.069099433720111847</v>
       </c>
       <c r="H9" s="1">
-        <v>7.006537914276123E-2</v>
+        <v>0.07006537914276123</v>
       </c>
       <c r="I9" s="1">
-        <v>6.5851092338562012E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.065851092338562012</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2735,25 +2735,25 @@
         <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>7.1771502494812012E-2</v>
+        <v>0.071771502494812012</v>
       </c>
       <c r="E10" s="1">
-        <v>7.7161580324172974E-2</v>
+        <v>0.077161580324172974</v>
       </c>
       <c r="F10" s="1">
-        <v>6.2606662511825562E-2</v>
+        <v>0.062606662511825562</v>
       </c>
       <c r="G10" s="1">
-        <v>6.7443951964378357E-2</v>
+        <v>0.067443951964378357</v>
       </c>
       <c r="H10" s="1">
-        <v>6.0106795281171799E-2</v>
+        <v>0.060106795281171799</v>
       </c>
       <c r="I10" s="1">
-        <v>7.6302647590637207E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.076302647590637207</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2764,25 +2764,25 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>6.6454246640205383E-2</v>
+        <v>0.066454246640205383</v>
       </c>
       <c r="E11" s="1">
-        <v>7.7107109129428864E-2</v>
+        <v>0.077107109129428864</v>
       </c>
       <c r="F11" s="1">
-        <v>5.7037819176912308E-2</v>
+        <v>0.057037819176912308</v>
       </c>
       <c r="G11" s="1">
-        <v>6.7771337926387787E-2</v>
+        <v>0.067771337926387787</v>
       </c>
       <c r="H11" s="1">
-        <v>5.0893060863018036E-2</v>
+        <v>0.050893060863018036</v>
       </c>
       <c r="I11" s="1">
-        <v>6.7591950297355652E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.067591950297355652</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2793,25 +2793,25 @@
         <v>20</v>
       </c>
       <c r="D12" s="1">
-        <v>8.4944598376750946E-2</v>
+        <v>0.084944598376750946</v>
       </c>
       <c r="E12" s="1">
-        <v>8.0988436937332153E-2</v>
+        <v>0.080988436937332153</v>
       </c>
       <c r="F12" s="1">
-        <v>7.2338446974754333E-2</v>
+        <v>0.072338446974754333</v>
       </c>
       <c r="G12" s="1">
-        <v>6.39185830950737E-2</v>
+        <v>0.0639185830950737</v>
       </c>
       <c r="H12" s="1">
-        <v>7.5108356773853302E-2</v>
+        <v>0.075108356773853302</v>
       </c>
       <c r="I12" s="1">
-        <v>6.0554653406143188E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.060554653406143189</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2822,25 +2822,25 @@
         <v>13</v>
       </c>
       <c r="D13" s="1">
-        <v>8.0126367509365082E-2</v>
+        <v>0.080126367509365082</v>
       </c>
       <c r="E13" s="1">
-        <v>8.3253808319568634E-2</v>
+        <v>0.083253808319568634</v>
       </c>
       <c r="F13" s="1">
-        <v>6.5562218427658081E-2</v>
+        <v>0.065562218427658081</v>
       </c>
       <c r="G13" s="1">
-        <v>6.5047271549701691E-2</v>
+        <v>0.065047271549701691</v>
       </c>
       <c r="H13" s="1">
-        <v>6.1024479568004608E-2</v>
+        <v>0.061024479568004608</v>
       </c>
       <c r="I13" s="1">
-        <v>6.0167685151100159E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.060167685151100159</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2851,25 +2851,25 @@
         <v>20</v>
       </c>
       <c r="D14" s="1">
-        <v>7.6071277260780334E-2</v>
+        <v>0.076071277260780335</v>
       </c>
       <c r="E14" s="1">
-        <v>8.0935738980770111E-2</v>
+        <v>0.080935738980770111</v>
       </c>
       <c r="F14" s="1">
-        <v>6.6357851028442383E-2</v>
+        <v>0.066357851028442383</v>
       </c>
       <c r="G14" s="1">
-        <v>6.9757610559463501E-2</v>
+        <v>0.069757610559463501</v>
       </c>
       <c r="H14" s="1">
-        <v>6.8064190447330475E-2</v>
+        <v>0.068064190447330475</v>
       </c>
       <c r="I14" s="1">
-        <v>7.2722166776657104E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.072722166776657104</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2880,25 +2880,25 @@
         <v>13</v>
       </c>
       <c r="D15" s="1">
-        <v>7.1175716817378998E-2</v>
+        <v>0.071175716817378998</v>
       </c>
       <c r="E15" s="1">
-        <v>7.8463777899742126E-2</v>
+        <v>0.078463777899742127</v>
       </c>
       <c r="F15" s="1">
-        <v>5.8435861021280289E-2</v>
+        <v>0.058435861021280289</v>
       </c>
       <c r="G15" s="1">
-        <v>6.6548466682434082E-2</v>
+        <v>0.066548466682434082</v>
       </c>
       <c r="H15" s="1">
-        <v>5.266648530960083E-2</v>
+        <v>0.05266648530960083</v>
       </c>
       <c r="I15" s="1">
-        <v>6.6213987767696381E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.066213987767696381</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2909,25 +2909,25 @@
         <v>20</v>
       </c>
       <c r="D16" s="1">
-        <v>6.5936900675296783E-2</v>
+        <v>0.065936900675296783</v>
       </c>
       <c r="E16" s="1">
-        <v>7.879175990819931E-2</v>
+        <v>0.07879175990819931</v>
       </c>
       <c r="F16" s="1">
-        <v>5.9424165636301041E-2</v>
+        <v>0.059424165636301041</v>
       </c>
       <c r="G16" s="1">
-        <v>6.5853461623191833E-2</v>
+        <v>0.065853461623191834</v>
       </c>
       <c r="H16" s="1">
-        <v>5.8515794575214386E-2</v>
+        <v>0.058515794575214386</v>
       </c>
       <c r="I16" s="1">
-        <v>7.7620796859264374E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.077620796859264374</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2938,25 +2938,25 @@
         <v>13</v>
       </c>
       <c r="D17" s="1">
-        <v>6.0066677629947662E-2</v>
+        <v>0.060066677629947662</v>
       </c>
       <c r="E17" s="1">
-        <v>7.4729807674884796E-2</v>
+        <v>0.074729807674884796</v>
       </c>
       <c r="F17" s="1">
-        <v>5.1649007946252823E-2</v>
+        <v>0.051649007946252823</v>
       </c>
       <c r="G17" s="1">
-        <v>6.3189737498760223E-2</v>
+        <v>0.063189737498760223</v>
       </c>
       <c r="H17" s="1">
-        <v>4.7169208526611328E-2</v>
+        <v>0.047169208526611328</v>
       </c>
       <c r="I17" s="1">
-        <v>5.9751883149147034E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.059751883149147034</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2967,25 +2967,25 @@
         <v>20</v>
       </c>
       <c r="D18" s="1">
-        <v>7.3303773999214172E-2</v>
+        <v>0.073303773999214172</v>
       </c>
       <c r="E18" s="1">
-        <v>7.3518984019756317E-2</v>
+        <v>0.073518984019756317</v>
       </c>
       <c r="F18" s="1">
-        <v>6.5997079014778137E-2</v>
+        <v>0.065997079014778137</v>
       </c>
       <c r="G18" s="1">
-        <v>6.2627837061882019E-2</v>
+        <v>0.062627837061882019</v>
       </c>
       <c r="H18" s="1">
-        <v>6.009707972407341E-2</v>
+        <v>0.06009707972407341</v>
       </c>
       <c r="I18" s="1">
-        <v>5.6753363460302353E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.056753363460302353</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2996,25 +2996,25 @@
         <v>13</v>
       </c>
       <c r="D19" s="1">
-        <v>6.6943518817424774E-2</v>
+        <v>0.066943518817424774</v>
       </c>
       <c r="E19" s="1">
-        <v>7.3524676263332367E-2</v>
+        <v>0.073524676263332367</v>
       </c>
       <c r="F19" s="1">
-        <v>5.8979485183954239E-2</v>
+        <v>0.058979485183954239</v>
       </c>
       <c r="G19" s="1">
-        <v>6.3168913125991821E-2</v>
+        <v>0.063168913125991821</v>
       </c>
       <c r="H19" s="1">
-        <v>4.8897575587034225E-2</v>
+        <v>0.048897575587034226</v>
       </c>
       <c r="I19" s="1">
-        <v>5.3211066871881485E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.053211066871881485</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -3025,25 +3025,25 @@
         <v>20</v>
       </c>
       <c r="D20" s="1">
-        <v>7.9999998211860657E-2</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="E20" s="1">
         <v>0.10224657505750656</v>
       </c>
       <c r="F20" s="1">
-        <v>6.8683475255966187E-2</v>
+        <v>0.068683475255966187</v>
       </c>
       <c r="G20" s="1">
-        <v>9.4621852040290833E-2</v>
+        <v>0.094621852040290833</v>
       </c>
       <c r="H20" s="1">
-        <v>6.007617712020874E-2</v>
+        <v>0.06007617712020874</v>
       </c>
       <c r="I20" s="1">
-        <v>9.1132178902626038E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.091132178902626038</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -3054,22 +3054,22 @@
         <v>13</v>
       </c>
       <c r="D21" s="1">
-        <v>7.8719623386859894E-2</v>
+        <v>0.078719623386859894</v>
       </c>
       <c r="E21" s="1">
-        <v>9.5909900963306427E-2</v>
+        <v>0.095909900963306427</v>
       </c>
       <c r="F21" s="1">
-        <v>6.8595185875892639E-2</v>
+        <v>0.068595185875892639</v>
       </c>
       <c r="G21" s="1">
-        <v>8.5455283522605896E-2</v>
+        <v>0.085455283522605896</v>
       </c>
       <c r="H21" s="1">
-        <v>5.6506790220737457E-2</v>
+        <v>0.056506790220737457</v>
       </c>
       <c r="I21" s="1">
-        <v>8.5216939449310303E-2</v>
+        <v>0.085216939449310303</v>
       </c>
     </row>
   </sheetData>
@@ -3078,16 +3078,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3127,25 +3127,25 @@
         <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>6.0732025653123856E-2</v>
+        <v>0.05617465078830719</v>
       </c>
       <c r="E2" s="1">
-        <v>6.4069397747516632E-2</v>
+        <v>0.057825334370136261</v>
       </c>
       <c r="F2" s="1">
-        <v>5.2527051419019699E-2</v>
+        <v>0.048352934420108795</v>
       </c>
       <c r="G2" s="1">
-        <v>5.6110400706529617E-2</v>
+        <v>0.051224928349256516</v>
       </c>
       <c r="H2" s="1">
-        <v>4.8739612102508545E-2</v>
+        <v>0.044458888471126556</v>
       </c>
       <c r="I2" s="1">
-        <v>6.1221208423376083E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.058053623884916306</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3156,25 +3156,25 @@
         <v>21</v>
       </c>
       <c r="D3" s="1">
-        <v>5.9880614280700684E-2</v>
+        <v>0.05160946398973465</v>
       </c>
       <c r="E3" s="1">
-        <v>6.3190922141075134E-2</v>
+        <v>0.057790115475654602</v>
       </c>
       <c r="F3" s="1">
-        <v>4.8060748726129532E-2</v>
+        <v>0.041228320449590683</v>
       </c>
       <c r="G3" s="1">
-        <v>5.7693563401699066E-2</v>
+        <v>0.05243450403213501</v>
       </c>
       <c r="H3" s="1">
-        <v>5.4175112396478653E-2</v>
+        <v>0.051078867167234421</v>
       </c>
       <c r="I3" s="1">
-        <v>7.1508444845676422E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.064578674733638763</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3185,25 +3185,25 @@
         <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>7.0509985089302063E-2</v>
+        <v>0.061516165733337402</v>
       </c>
       <c r="E4" s="1">
-        <v>7.4239104986190796E-2</v>
+        <v>0.069500997662544251</v>
       </c>
       <c r="F4" s="1">
-        <v>5.553654208779335E-2</v>
+        <v>0.048263438045978546</v>
       </c>
       <c r="G4" s="1">
-        <v>6.6033616662025452E-2</v>
+        <v>0.061694487929344177</v>
       </c>
       <c r="H4" s="1">
-        <v>6.2092546373605728E-2</v>
+        <v>0.059073105454444885</v>
       </c>
       <c r="I4" s="1">
-        <v>7.6222792267799377E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.073380261659622192</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3214,25 +3214,25 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>4.7510087490081787E-2</v>
+        <v>0.042013496160507202</v>
       </c>
       <c r="E5" s="1">
-        <v>4.6024877578020096E-2</v>
+        <v>0.038818981498479843</v>
       </c>
       <c r="F5" s="1">
-        <v>4.2881600558757782E-2</v>
+        <v>0.039875678718090057</v>
       </c>
       <c r="G5" s="1">
-        <v>3.2254632562398911E-2</v>
+        <v>0.027170538902282715</v>
       </c>
       <c r="H5" s="1">
-        <v>4.750530794262886E-2</v>
+        <v>0.042717762291431427</v>
       </c>
       <c r="I5" s="1">
-        <v>4.9081113189458847E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.045453578233718872</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3243,25 +3243,25 @@
         <v>21</v>
       </c>
       <c r="D6" s="1">
-        <v>5.194174125790596E-2</v>
+        <v>0.043668478727340698</v>
       </c>
       <c r="E6" s="1">
-        <v>4.6674016863107681E-2</v>
+        <v>0.040553078055381775</v>
       </c>
       <c r="F6" s="1">
-        <v>4.0865179151296616E-2</v>
+        <v>0.034268669784069061</v>
       </c>
       <c r="G6" s="1">
-        <v>4.0115982294082642E-2</v>
+        <v>0.034138523042201996</v>
       </c>
       <c r="H6" s="1">
-        <v>5.0596162676811218E-2</v>
+        <v>0.046879116445779801</v>
       </c>
       <c r="I6" s="1">
-        <v>4.560474306344986E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.041988909244537354</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3272,25 +3272,25 @@
         <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>4.7710075974464417E-2</v>
+        <v>0.041713923215866089</v>
       </c>
       <c r="E7" s="1">
-        <v>4.7753609716892242E-2</v>
+        <v>0.040620841085910797</v>
       </c>
       <c r="F7" s="1">
-        <v>3.8968700915575027E-2</v>
+        <v>0.034140396863222122</v>
       </c>
       <c r="G7" s="1">
-        <v>4.1586827486753464E-2</v>
+        <v>0.036069039255380631</v>
       </c>
       <c r="H7" s="1">
-        <v>4.6862687915563583E-2</v>
+        <v>0.043224930763244629</v>
       </c>
       <c r="I7" s="1">
-        <v>5.0730876624584198E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.045515932142734528</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3301,25 +3301,25 @@
         <v>13</v>
       </c>
       <c r="D8" s="1">
-        <v>5.705849826335907E-2</v>
+        <v>0.05231596902012825</v>
       </c>
       <c r="E8" s="1">
-        <v>6.4845055341720581E-2</v>
+        <v>0.0575077123939991</v>
       </c>
       <c r="F8" s="1">
-        <v>5.3781557828187943E-2</v>
+        <v>0.049347363412380219</v>
       </c>
       <c r="G8" s="1">
-        <v>5.8977626264095306E-2</v>
+        <v>0.051951088011264801</v>
       </c>
       <c r="H8" s="1">
-        <v>5.7844016700983047E-2</v>
+        <v>0.054232250899076462</v>
       </c>
       <c r="I8" s="1">
-        <v>6.3354134559631348E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.060018967837095261</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3327,28 +3327,28 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
-        <v>8.3923906087875366E-2</v>
+        <v>0.066813893616199493</v>
       </c>
       <c r="E9" s="1">
-        <v>7.1903564035892487E-2</v>
+        <v>0.057924751192331314</v>
       </c>
       <c r="F9" s="1">
-        <v>7.7888064086437225E-2</v>
+        <v>0.062374264001846313</v>
       </c>
       <c r="G9" s="1">
-        <v>5.5073957890272141E-2</v>
+        <v>0.047444775700569153</v>
       </c>
       <c r="H9" s="1">
-        <v>8.9838892221450806E-2</v>
+        <v>0.078170418739318848</v>
       </c>
       <c r="I9" s="1">
-        <v>6.373528391122818E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.052892241626977921</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3356,28 +3356,28 @@
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>7.296154648065567E-2</v>
+        <v>0.078097611665725708</v>
       </c>
       <c r="E10" s="1">
-        <v>6.6890202462673187E-2</v>
+        <v>0.06375441700220108</v>
       </c>
       <c r="F10" s="1">
-        <v>6.8472199141979218E-2</v>
+        <v>0.072186104953289032</v>
       </c>
       <c r="G10" s="1">
-        <v>5.477578192949295E-2</v>
+        <v>0.048510834574699402</v>
       </c>
       <c r="H10" s="1">
-        <v>8.2802049815654755E-2</v>
+        <v>0.08697471022605896</v>
       </c>
       <c r="I10" s="1">
-        <v>5.6489013135433197E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.059970732778310776</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3388,25 +3388,25 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>4.4097885489463806E-2</v>
+        <v>0.039386335760354996</v>
       </c>
       <c r="E11" s="1">
-        <v>5.3952474147081375E-2</v>
+        <v>0.047454960644245148</v>
       </c>
       <c r="F11" s="1">
-        <v>4.1145507246255875E-2</v>
+        <v>0.037053413689136505</v>
       </c>
       <c r="G11" s="1">
-        <v>4.8246316611766815E-2</v>
+        <v>0.042851705104112625</v>
       </c>
       <c r="H11" s="1">
-        <v>4.5561544597148895E-2</v>
+        <v>0.042719796299934387</v>
       </c>
       <c r="I11" s="1">
-        <v>5.8649804443120956E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.055612068623304367</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3417,25 +3417,25 @@
         <v>21</v>
       </c>
       <c r="D12" s="1">
-        <v>4.4156964868307114E-2</v>
+        <v>0.039367526769638062</v>
       </c>
       <c r="E12" s="1">
-        <v>4.9160003662109375E-2</v>
+        <v>0.04078688845038414</v>
       </c>
       <c r="F12" s="1">
-        <v>4.0142346173524857E-2</v>
+        <v>0.036130271852016449</v>
       </c>
       <c r="G12" s="1">
-        <v>4.464271292090416E-2</v>
+        <v>0.036443993449211121</v>
       </c>
       <c r="H12" s="1">
-        <v>4.99735027551651E-2</v>
+        <v>0.047341573983430862</v>
       </c>
       <c r="I12" s="1">
-        <v>5.392015352845192E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.05091317743062973</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3446,25 +3446,25 @@
         <v>20</v>
       </c>
       <c r="D13" s="1">
-        <v>4.9888614565134048E-2</v>
+        <v>0.045784421265125275</v>
       </c>
       <c r="E13" s="1">
-        <v>4.9288969486951828E-2</v>
+        <v>0.039934225380420685</v>
       </c>
       <c r="F13" s="1">
-        <v>4.4964388012886047E-2</v>
+        <v>0.041493140161037445</v>
       </c>
       <c r="G13" s="1">
-        <v>4.5427627861499786E-2</v>
+        <v>0.035399135202169418</v>
       </c>
       <c r="H13" s="1">
-        <v>5.9658464044332504E-2</v>
+        <v>0.056529216468334198</v>
       </c>
       <c r="I13" s="1">
-        <v>5.5496521294116974E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.051557201892137528</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3475,25 +3475,25 @@
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <v>5.704064667224884E-2</v>
+        <v>0.052954886108636856</v>
       </c>
       <c r="E14" s="1">
-        <v>6.5429180860519409E-2</v>
+        <v>0.053868982940912247</v>
       </c>
       <c r="F14" s="1">
-        <v>5.4214578121900558E-2</v>
+        <v>0.049771510064601898</v>
       </c>
       <c r="G14" s="1">
-        <v>5.4118726402521133E-2</v>
+        <v>0.044556263834238052</v>
       </c>
       <c r="H14" s="1">
-        <v>5.2657000720500946E-2</v>
+        <v>0.051361732184886932</v>
       </c>
       <c r="I14" s="1">
-        <v>5.5641300976276398E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.049950111657381058</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3501,28 +3501,28 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1">
-        <v>7.6325781643390656E-2</v>
+        <v>0.059178154915571213</v>
       </c>
       <c r="E15" s="1">
-        <v>7.7417343854904175E-2</v>
+        <v>0.056496087461709976</v>
       </c>
       <c r="F15" s="1">
-        <v>6.8105906248092651E-2</v>
+        <v>0.052232503890991211</v>
       </c>
       <c r="G15" s="1">
-        <v>5.8709755539894104E-2</v>
+        <v>0.044814392924308777</v>
       </c>
       <c r="H15" s="1">
-        <v>7.1009114384651184E-2</v>
+        <v>0.054016690701246262</v>
       </c>
       <c r="I15" s="1">
-        <v>6.0378029942512512E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.052172701805830002</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3530,28 +3530,28 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1">
-        <v>6.5405286848545074E-2</v>
+        <v>0.070727154612541199</v>
       </c>
       <c r="E16" s="1">
-        <v>6.489437073469162E-2</v>
+        <v>0.064735077321529388</v>
       </c>
       <c r="F16" s="1">
-        <v>5.6690040975809097E-2</v>
+        <v>0.064169019460678101</v>
       </c>
       <c r="G16" s="1">
-        <v>5.1428485661745071E-2</v>
+        <v>0.049849245697259903</v>
       </c>
       <c r="H16" s="1">
-        <v>5.6045219302177429E-2</v>
+        <v>0.068740174174308777</v>
       </c>
       <c r="I16" s="1">
-        <v>5.5317871272563934E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.056195486336946488</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -3562,25 +3562,25 @@
         <v>20</v>
       </c>
       <c r="D17" s="1">
-        <v>4.4503450393676758E-2</v>
+        <v>0.040310077369213104</v>
       </c>
       <c r="E17" s="1">
-        <v>6.6861391067504883E-2</v>
+        <v>0.067308209836483002</v>
       </c>
       <c r="F17" s="1">
-        <v>3.7157908082008362E-2</v>
+        <v>0.034843768924474716</v>
       </c>
       <c r="G17" s="1">
-        <v>7.0327058434486389E-2</v>
+        <v>0.070556610822677612</v>
       </c>
       <c r="H17" s="1">
-        <v>6.6452436149120331E-2</v>
+        <v>0.067878447473049164</v>
       </c>
       <c r="I17" s="1">
-        <v>0.10627821832895279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.098924554884433746</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3591,25 +3591,25 @@
         <v>21</v>
       </c>
       <c r="D18" s="1">
-        <v>4.6778228133916855E-2</v>
+        <v>0.041196983307600021</v>
       </c>
       <c r="E18" s="1">
-        <v>6.535840779542923E-2</v>
+        <v>0.059329647570848465</v>
       </c>
       <c r="F18" s="1">
-        <v>3.6049086600542068E-2</v>
+        <v>0.03178974986076355</v>
       </c>
       <c r="G18" s="1">
-        <v>5.5035486817359924E-2</v>
+        <v>0.050676636397838593</v>
       </c>
       <c r="H18" s="1">
-        <v>4.7781337052583694E-2</v>
+        <v>0.046695537865161896</v>
       </c>
       <c r="I18" s="1">
-        <v>8.0280661582946777E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.071552000939846039</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -3620,25 +3620,25 @@
         <v>13</v>
       </c>
       <c r="D19" s="1">
-        <v>5.1039338111877441E-2</v>
+        <v>0.044602975249290466</v>
       </c>
       <c r="E19" s="1">
-        <v>5.1845591515302658E-2</v>
+        <v>0.047365710139274597</v>
       </c>
       <c r="F19" s="1">
-        <v>4.3775744736194611E-2</v>
+        <v>0.036901488900184631</v>
       </c>
       <c r="G19" s="1">
-        <v>4.4726189225912094E-2</v>
+        <v>0.041045889258384705</v>
       </c>
       <c r="H19" s="1">
-        <v>4.6210054308176041E-2</v>
+        <v>0.044777132570743561</v>
       </c>
       <c r="I19" s="1">
-        <v>5.4432656615972519E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.051692120730876923</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -3649,25 +3649,25 @@
         <v>20</v>
       </c>
       <c r="D20" s="1">
-        <v>5.4776258766651154E-2</v>
+        <v>0.047015395015478134</v>
       </c>
       <c r="E20" s="1">
-        <v>6.5786689519882202E-2</v>
+        <v>0.061984565109014511</v>
       </c>
       <c r="F20" s="1">
-        <v>5.1235366612672806E-2</v>
+        <v>0.04625726118683815</v>
       </c>
       <c r="G20" s="1">
-        <v>5.9989694505929947E-2</v>
+        <v>0.057423654943704605</v>
       </c>
       <c r="H20" s="1">
-        <v>5.2455045282840729E-2</v>
+        <v>0.050053652375936508</v>
       </c>
       <c r="I20" s="1">
-        <v>8.2657575607299805E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.082157902419567108</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -3678,25 +3678,25 @@
         <v>21</v>
       </c>
       <c r="D21" s="1">
-        <v>4.8938725143671036E-2</v>
+        <v>0.04233773797750473</v>
       </c>
       <c r="E21" s="1">
-        <v>5.9204187244176865E-2</v>
+        <v>0.054828748106956482</v>
       </c>
       <c r="F21" s="1">
-        <v>4.3642893433570862E-2</v>
+        <v>0.039202205836772919</v>
       </c>
       <c r="G21" s="1">
-        <v>5.2675057202577591E-2</v>
+        <v>0.049602121114730835</v>
       </c>
       <c r="H21" s="1">
-        <v>4.6159025281667709E-2</v>
+        <v>0.043669760227203369</v>
       </c>
       <c r="I21" s="1">
-        <v>7.3792897164821625E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.072661422193050385</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -3707,25 +3707,25 @@
         <v>13</v>
       </c>
       <c r="D22" s="1">
-        <v>5.2134677767753601E-2</v>
+        <v>0.047477968037128448</v>
       </c>
       <c r="E22" s="1">
-        <v>5.8615777641534805E-2</v>
+        <v>0.051074277609586716</v>
       </c>
       <c r="F22" s="1">
-        <v>4.8298884183168411E-2</v>
+        <v>0.043819610029459</v>
       </c>
       <c r="G22" s="1">
-        <v>5.2163608372211456E-2</v>
+        <v>0.046039242297410965</v>
       </c>
       <c r="H22" s="1">
-        <v>4.6609316021203995E-2</v>
+        <v>0.044349163770675659</v>
       </c>
       <c r="I22" s="1">
-        <v>5.5301066488027573E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.051638633012771607</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -3736,25 +3736,25 @@
         <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>5.5787641555070877E-2</v>
+        <v>0.049226097762584686</v>
       </c>
       <c r="E23" s="1">
-        <v>5.564223974943161E-2</v>
+        <v>0.047770112752914429</v>
       </c>
       <c r="F23" s="1">
-        <v>4.9797490239143372E-2</v>
+        <v>0.04465118795633316</v>
       </c>
       <c r="G23" s="1">
-        <v>4.6220831573009491E-2</v>
+        <v>0.040601871907711029</v>
       </c>
       <c r="H23" s="1">
-        <v>5.0142049789428711E-2</v>
+        <v>0.047669019550085068</v>
       </c>
       <c r="I23" s="1">
-        <v>4.9882706254720688E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.046178668737411499</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -3765,22 +3765,22 @@
         <v>20</v>
       </c>
       <c r="D24" s="1">
-        <v>6.030721589922905E-2</v>
+        <v>0.05383773148059845</v>
       </c>
       <c r="E24" s="1">
-        <v>5.7540323585271835E-2</v>
+        <v>0.049614924937486649</v>
       </c>
       <c r="F24" s="1">
-        <v>5.5324908345937729E-2</v>
+        <v>0.050557252019643784</v>
       </c>
       <c r="G24" s="1">
-        <v>4.8250313848257065E-2</v>
+        <v>0.042925860732793808</v>
       </c>
       <c r="H24" s="1">
-        <v>5.5123060941696167E-2</v>
+        <v>0.052826154977083206</v>
       </c>
       <c r="I24" s="1">
-        <v>5.2587557584047318E-2</v>
+        <v>0.049093399196863174</v>
       </c>
     </row>
   </sheetData>
@@ -3789,22 +3789,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C71F3F-6F9B-452C-A26D-1655F47F071E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C71F3F-6F9B-452C-A26D-1655F47F071E}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="6" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="16" customWidth="true"/>
+    <col min="9" max="9" width="17.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -3823,7 +3823,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -4123,13 +4123,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -4232,22 +4232,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2088C4D4-0018-40AE-9D8C-0F9A114E6116}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2088C4D4-0018-40AE-9D8C-0F9A114E6116}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="6" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="16" customWidth="true"/>
+    <col min="9" max="9" width="17.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -4344,7 +4344,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -4524,7 +4524,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -4588,13 +4588,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -4734,22 +4734,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CFC922-0F20-4A9F-906A-AECCCAD51B22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CFC922-0F20-4A9F-906A-AECCCAD51B22}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="6" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="16" customWidth="true"/>
+    <col min="9" max="9" width="17.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -4835,7 +4835,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -5004,7 +5004,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -5075,13 +5075,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>19</v>
       </c>
@@ -5184,22 +5184,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5D74C1-4B06-45DE-9DF5-952ADBD2B8F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5D74C1-4B06-45DE-9DF5-952ADBD2B8F2}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="6" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="16" customWidth="true"/>
+    <col min="9" max="9" width="17.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>44</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -5296,7 +5296,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -5472,7 +5472,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -5534,13 +5534,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>27</v>
       </c>

</xml_diff>